<commit_message>
diff layout for admin
</commit_message>
<xml_diff>
--- a/Pic dimension.xlsx
+++ b/Pic dimension.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-32000" yWindow="0" windowWidth="32000" windowHeight="18000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -401,7 +401,7 @@
       </c>
       <c r="I1">
         <f>I2*H1/H2</f>
-        <v>145.02074688796679</v>
+        <v>87.012448132780079</v>
       </c>
     </row>
     <row r="2" spans="6:9" x14ac:dyDescent="0.2">
@@ -415,7 +415,7 @@
         <v>482</v>
       </c>
       <c r="I2">
-        <v>50</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>